<commit_message>
Agregado funcion de continuar
</commit_message>
<xml_diff>
--- a/book_150_200.xlsx
+++ b/book_150_200.xlsx
@@ -205,11 +205,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,7 +233,7 @@
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -267,7 +267,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="1" width="10.9"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="10.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>